<commit_message>
Updated the code to provide screen scraping works for Sainsburys store
</commit_message>
<xml_diff>
--- a/pricecomparison/pricewatch.xlsx
+++ b/pricecomparison/pricewatch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivek/Development/price-compare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03887716-6161-4C44-83AF-FEE81F40F927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA9A93C-7FA9-F044-BC77-558AC478D7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Product Name</t>
   </si>
@@ -66,24 +66,58 @@
   </si>
   <si>
     <t>https://www.sainsburys.co.uk/groceries-api/gol-services/product/v1/product?filter[product_seo_url]=gb%2Fgroceries%2Fall-household-essentials%2Ffairy-liquid-platinum-650ml</t>
+  </si>
+  <si>
+    <t>Sainsbury's Whole Cucumber</t>
+  </si>
+  <si>
+    <t>Sainsbury's Fairtrade Bananas x5</t>
+  </si>
+  <si>
+    <t>Sainsbury's Mixed Peppers, SO Organic x3 (Colours may vary)</t>
+  </si>
+  <si>
+    <t>Sainsbury's Strawberries 400g</t>
+  </si>
+  <si>
+    <t>Sainsbury's Easy Peelers, Taste the Difference 600g</t>
+  </si>
+  <si>
+    <t>Sainsbury's British Baby Potatoes 1kg</t>
+  </si>
+  <si>
+    <t>Sainsbury's Limes</t>
+  </si>
+  <si>
+    <t>Sainsbury's Aubergine</t>
+  </si>
+  <si>
+    <t>Sainsbury's Baby Button Mushrooms 200g</t>
+  </si>
+  <si>
+    <t>Sainsbury's Young Spinach 260g</t>
+  </si>
+  <si>
+    <t>Sainsbury's Root Ginger Loose</t>
+  </si>
+  <si>
+    <t>Sainsbury's Cherry Tomatoes 500g</t>
+  </si>
+  <si>
+    <t>Sainsbury's Fresh Packed Coriander 100g</t>
+  </si>
+  <si>
+    <t>PG tips Original Biodegradable Black Tea Bags x240</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -127,19 +161,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -452,10 +484,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -465,13 +497,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -523,7 +555,7 @@
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
       <c r="C6">
@@ -534,7 +566,7 @@
       <c r="A7" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" t="s">
         <v>4</v>
       </c>
       <c r="C7">
@@ -545,8 +577,78 @@
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
@@ -554,8 +656,14 @@
     <hyperlink ref="B6" r:id="rId1" xr:uid="{4B8C0A48-B37C-8642-B9A4-20FD56D21664}"/>
     <hyperlink ref="B7" r:id="rId2" xr:uid="{0EEECC29-9043-1945-B396-9C8553B8741A}"/>
     <hyperlink ref="B8" r:id="rId3" xr:uid="{38609013-2FAC-D64B-8A6D-1D5BA7182200}"/>
+    <hyperlink ref="A18" r:id="rId4" display="https://www.sainsburys.co.uk/shop/gb/groceries/product/details/fruitandveg-essentials/sainsburys-young-spinach-260g" xr:uid="{C3F64C88-80FF-5548-8499-FB0F51FDA895}"/>
+    <hyperlink ref="A19" r:id="rId5" display="https://www.sainsburys.co.uk/shop/gb/groceries/product/details/fruitandveg-essentials/sainsburys-root-ginger-loose" xr:uid="{E07DB969-2432-C440-BB47-9BA1FC6C063A}"/>
+    <hyperlink ref="A20" r:id="rId6" display="https://www.sainsburys.co.uk/shop/gb/groceries/product/details/fruitandveg-essentials/sainsburys-cherry-tomatoes-500g" xr:uid="{9F9A90C0-BDD6-3942-AAD8-EB187978ADA9}"/>
+    <hyperlink ref="A21" r:id="rId7" display="https://www.sainsburys.co.uk/shop/gb/groceries/product/details/fruitandveg-essentials/sainsburys-fresh-coriander-100g" xr:uid="{9F2C4499-C9E5-CE49-A924-16D8A2E72819}"/>
+    <hyperlink ref="A22" r:id="rId8" display="https://www.sainsburys.co.uk/shop/gb/groceries/product/details/food-cupboard-essentials/pg-tips-pyramid-tea-bags-x240" xr:uid="{AFDD1319-AFA9-3546-A0F1-25238BDDB839}"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added new store check
</commit_message>
<xml_diff>
--- a/pricecomparison/pricewatch.xlsx
+++ b/pricecomparison/pricewatch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10303"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10403"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivek/Development/price-compare/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivek/Development/pricecomparison/pricecomparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DA9A93C-7FA9-F044-BC77-558AC478D7E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE7BE0FD-6CD6-2343-952B-730A355753B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sainsburys" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>Product Name</t>
   </si>
@@ -68,12 +68,12 @@
     <t>https://www.sainsburys.co.uk/groceries-api/gol-services/product/v1/product?filter[product_seo_url]=gb%2Fgroceries%2Fall-household-essentials%2Ffairy-liquid-platinum-650ml</t>
   </si>
   <si>
+    <t>Sainsbury's Fairtrade Bananas x5</t>
+  </si>
+  <si>
     <t>Sainsbury's Whole Cucumber</t>
   </si>
   <si>
-    <t>Sainsbury's Fairtrade Bananas x5</t>
-  </si>
-  <si>
     <t>Sainsbury's Mixed Peppers, SO Organic x3 (Colours may vary)</t>
   </si>
   <si>
@@ -108,6 +108,30 @@
   </si>
   <si>
     <t>PG tips Original Biodegradable Black Tea Bags x240</t>
+  </si>
+  <si>
+    <t>https://www.tesco.com/groceries/en-GB/products/261738730</t>
+  </si>
+  <si>
+    <t>https://www.tesco.com/groceries/en-GB/products/255000362</t>
+  </si>
+  <si>
+    <t>British Whole Milk 2.27L (4 pint)</t>
+  </si>
+  <si>
+    <t>British Whole Milk 3.4L (6 pint)</t>
+  </si>
+  <si>
+    <t>https://www.tesco.com/groceries/en-GB/products/255986260</t>
+  </si>
+  <si>
+    <t>https://www.tesco.com/groceries/en-GB/products/254656543</t>
+  </si>
+  <si>
+    <t>Tesco British Semi Skimmed Milk 2.272L 4 Pints</t>
+  </si>
+  <si>
+    <t>Tesco Semi Skimmed Milk 3.408L/6 Pints</t>
   </si>
 </sst>
 </file>
@@ -166,10 +190,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,24 +510,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5:B8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="52.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="195.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="151.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -580,88 +604,81 @@
       <c r="B8" t="s">
         <v>12</v>
       </c>
+      <c r="C8">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="2" t="s">
+      <c r="A11" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="2" t="s">
+      <c r="A14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="2" t="s">
+      <c r="A15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="2" t="s">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2" t="s">
+      <c r="A17" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2" t="s">
+      <c r="A18" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
+      <c r="A19" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2" t="s">
+      <c r="A20" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2" t="s">
+      <c r="A21" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2" t="s">
+      <c r="A22" t="s">
         <v>26</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1" xr:uid="{4B8C0A48-B37C-8642-B9A4-20FD56D21664}"/>
-    <hyperlink ref="B7" r:id="rId2" xr:uid="{0EEECC29-9043-1945-B396-9C8553B8741A}"/>
-    <hyperlink ref="B8" r:id="rId3" xr:uid="{38609013-2FAC-D64B-8A6D-1D5BA7182200}"/>
-    <hyperlink ref="A18" r:id="rId4" display="https://www.sainsburys.co.uk/shop/gb/groceries/product/details/fruitandveg-essentials/sainsburys-young-spinach-260g" xr:uid="{C3F64C88-80FF-5548-8499-FB0F51FDA895}"/>
-    <hyperlink ref="A19" r:id="rId5" display="https://www.sainsburys.co.uk/shop/gb/groceries/product/details/fruitandveg-essentials/sainsburys-root-ginger-loose" xr:uid="{E07DB969-2432-C440-BB47-9BA1FC6C063A}"/>
-    <hyperlink ref="A20" r:id="rId6" display="https://www.sainsburys.co.uk/shop/gb/groceries/product/details/fruitandveg-essentials/sainsburys-cherry-tomatoes-500g" xr:uid="{9F9A90C0-BDD6-3942-AAD8-EB187978ADA9}"/>
-    <hyperlink ref="A21" r:id="rId7" display="https://www.sainsburys.co.uk/shop/gb/groceries/product/details/fruitandveg-essentials/sainsburys-fresh-coriander-100g" xr:uid="{9F2C4499-C9E5-CE49-A924-16D8A2E72819}"/>
-    <hyperlink ref="A22" r:id="rId8" display="https://www.sainsburys.co.uk/shop/gb/groceries/product/details/food-cupboard-essentials/pg-tips-pyramid-tea-bags-x240" xr:uid="{AFDD1319-AFA9-3546-A0F1-25238BDDB839}"/>
-  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
@@ -729,15 +746,91 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.2000000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
-Adding Coop store -Add check if URL for product does not exist skip check -Added progress bar for all the stores -Minor cleanup
</commit_message>
<xml_diff>
--- a/pricecomparison/pricewatch.xlsx
+++ b/pricecomparison/pricewatch.xlsx
@@ -8,18 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivek/Development/price-compare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{DA3A5C66-B963-164A-B14D-2B107D8BA29A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{434F0B15-9092-A141-AA22-487503B482F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sainsburys" sheetId="1" r:id="rId1"/>
-    <sheet name="Tesco" sheetId="7" r:id="rId2"/>
-    <sheet name="Asda" sheetId="6" r:id="rId3"/>
-    <sheet name="Co-op" sheetId="2" r:id="rId4"/>
-    <sheet name="Ocado" sheetId="3" r:id="rId5"/>
-    <sheet name="Morissons" sheetId="4" r:id="rId6"/>
-    <sheet name="Lidl" sheetId="5" r:id="rId7"/>
+    <sheet name="Tesco" sheetId="2" r:id="rId2"/>
+    <sheet name="Asda" sheetId="3" r:id="rId3"/>
+    <sheet name="Co-op" sheetId="4" r:id="rId4"/>
+    <sheet name="Ocado" sheetId="5" r:id="rId5"/>
+    <sheet name="Morissons" sheetId="6" r:id="rId6"/>
+    <sheet name="Lidl" sheetId="7" r:id="rId7"/>
     <sheet name="M&amp;S" sheetId="8" r:id="rId8"/>
     <sheet name="Aldi" sheetId="9" r:id="rId9"/>
   </sheets>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
   <si>
     <t>Product Name</t>
   </si>
@@ -112,12 +112,60 @@
     <t>PG tips Original Biodegradable Black Tea Bags x240</t>
   </si>
   <si>
+    <t>https://www.tesco.com/groceries/en-GB/products/261738730</t>
+  </si>
+  <si>
+    <t>1.00</t>
+  </si>
+  <si>
+    <t>https://www.tesco.com/groceries/en-GB/products/255000362</t>
+  </si>
+  <si>
+    <t>1.10</t>
+  </si>
+  <si>
+    <t>Tesco British Semi Skimmed Milk 2.272L 4 Pints</t>
+  </si>
+  <si>
+    <t>https://www.tesco.com/groceries/en-GB/products/254656543</t>
+  </si>
+  <si>
+    <t>1.25</t>
+  </si>
+  <si>
+    <t>Tesco Whole Milk 2.27L (4 pint)</t>
+  </si>
+  <si>
+    <t>https://www.tesco.com/groceries/en-GB/products/254656399</t>
+  </si>
+  <si>
+    <t>Tesco Semi Skimmed Milk 3.408L/6 Pints</t>
+  </si>
+  <si>
+    <t>https://www.tesco.com/groceries/en-GB/products/255986260</t>
+  </si>
+  <si>
+    <t>1.70</t>
+  </si>
+  <si>
+    <t>Tesco Whole Milk 3.4L (6 pint)</t>
+  </si>
+  <si>
+    <t>https://www.tesco.com/groceries/en-GB/products/254957550</t>
+  </si>
+  <si>
+    <t>Fairy Platinum Quick Wash Washing Up Liquid 820ml</t>
+  </si>
+  <si>
+    <t>https://www.tesco.com/groceries/en-GB/products/311424196</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
     <t>https://groceries.asda.com/product/half-half-bread/kingsmill-medium-50-50-bread/42747407</t>
   </si>
   <si>
-    <t>1.10</t>
-  </si>
-  <si>
     <t>https://groceries.asda.com/product/wholemeal-bread/hovis-medium-wholemeal-bread/24742</t>
   </si>
   <si>
@@ -127,9 +175,6 @@
     <t>https://groceries.asda.com/product/semi-skimmed-milk/asda-semi-skimmed-milk/20504</t>
   </si>
   <si>
-    <t>1.25</t>
-  </si>
-  <si>
     <t>Asda Whole Milk 2.27L (4 pint)</t>
   </si>
   <si>
@@ -142,9 +187,6 @@
     <t>https://groceries.asda.com/product/semi-skimmed-milk/asda-semi-skimmed-milk/20506</t>
   </si>
   <si>
-    <t>1.70</t>
-  </si>
-  <si>
     <t>Asda Whole Milk 3.4L (6 pint)</t>
   </si>
   <si>
@@ -157,59 +199,35 @@
     <t>https://groceries.asda.com/product/washing-up-liquid/fairy-platinum-quickwash-original-washing-up-liquid-with-up-to-3-x-faster-tough-grease-cleaning/1000360714103</t>
   </si>
   <si>
-    <t>2.00</t>
-  </si>
-  <si>
-    <t>https://www.tesco.com/groceries/en-GB/products/261738730</t>
-  </si>
-  <si>
-    <t>1.00</t>
-  </si>
-  <si>
-    <t>https://www.tesco.com/groceries/en-GB/products/255000362</t>
-  </si>
-  <si>
-    <t>Tesco British Semi Skimmed Milk 2.272L 4 Pints</t>
-  </si>
-  <si>
-    <t>https://www.tesco.com/groceries/en-GB/products/254656543</t>
-  </si>
-  <si>
-    <t>Tesco Whole Milk 2.27L (4 pint)</t>
-  </si>
-  <si>
-    <t>https://www.tesco.com/groceries/en-GB/products/254656399</t>
-  </si>
-  <si>
-    <t>Tesco Semi Skimmed Milk 3.408L/6 Pints</t>
-  </si>
-  <si>
-    <t>https://www.tesco.com/groceries/en-GB/products/255986260</t>
-  </si>
-  <si>
-    <t>Tesco Whole Milk 3.4L (6 pint)</t>
-  </si>
-  <si>
-    <t>https://www.tesco.com/groceries/en-GB/products/254957550</t>
-  </si>
-  <si>
-    <t>Fairy Platinum Quick Wash Washing Up Liquid 820ml</t>
-  </si>
-  <si>
-    <t>https://www.tesco.com/groceries/en-GB/products/311424196</t>
+    <t>Co Op British Fresh Semi-Skimmed Milk 4 Pints/2.272L</t>
+  </si>
+  <si>
+    <t>https://api.shop.coop.co.uk/products/details/b91efa3f-d4a4-4b07-a991-886ce2f4e775?store_id=d8ad1898-e156-4c58-9386-f96d611d31eb</t>
+  </si>
+  <si>
+    <t>Co Op British Fresh Whole Milk 4 Pints/2.272L</t>
+  </si>
+  <si>
+    <t>https://api.shop.coop.co.uk/products/details/e3c61eda-a029-45ce-99f3-84ba9a8afa04?store_id=17eda196-0394-4cf5-9053-a7652fc76671</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -238,7 +256,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -291,11 +309,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -305,6 +338,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -798,7 +834,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -827,10 +863,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -838,65 +874,65 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>46</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="B5" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="C5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B7" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
   </sheetData>
@@ -906,17 +942,17 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="144.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="144.6640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -935,10 +971,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -946,65 +982,144 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>29</v>
+        <v>45</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C5" t="s">
         <v>33</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" t="s">
         <v>38</v>
-      </c>
-      <c r="B7" t="s">
-        <v>39</v>
-      </c>
-      <c r="C7" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="118" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" t="s">
+        <v>57</v>
+      </c>
+      <c r="C4">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>
@@ -1012,8 +1127,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1024,8 +1139,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1036,20 +1151,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated Excel & README
</commit_message>
<xml_diff>
--- a/pricecomparison/pricewatch.xlsx
+++ b/pricecomparison/pricewatch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivek/Development/price-compare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{434F0B15-9092-A141-AA22-487503B482F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6B4697-3FDD-F146-A8A3-E395359884FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,12 +24,11 @@
     <sheet name="Aldi" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="60">
   <si>
     <t>Product Name</t>
   </si>
@@ -1054,7 +1053,7 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1124,65 +1123,385 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
- Add OcadoΩ - Added logging - Updated README
</commit_message>
<xml_diff>
--- a/pricecomparison/pricewatch.xlsx
+++ b/pricecomparison/pricewatch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivek/Development/price-compare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD6B4697-3FDD-F146-A8A3-E395359884FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{96EC470F-E373-CB43-81FC-72A83A1E781C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sainsburys" sheetId="1" r:id="rId1"/>
@@ -24,11 +24,12 @@
     <sheet name="Aldi" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="66">
   <si>
     <t>Product Name</t>
   </si>
@@ -208,19 +209,43 @@
   </si>
   <si>
     <t>https://api.shop.coop.co.uk/products/details/e3c61eda-a029-45ce-99f3-84ba9a8afa04?store_id=17eda196-0394-4cf5-9053-a7652fc76671</t>
+  </si>
+  <si>
+    <t>https://www.ocado.com/products/hovis-tasty-wholemeal-medium-sliced-bread-15885011</t>
+  </si>
+  <si>
+    <t>1.20</t>
+  </si>
+  <si>
+    <t>Hovis Tasty Wholemeal Medium Sliced Bread 800g</t>
+  </si>
+  <si>
+    <t>Ocado British Semi Skimmed Milk 4 Pints</t>
+  </si>
+  <si>
+    <t>https://www.ocado.com/products/ocado-british-semi-skimmed-milk-4-pints-78914011</t>
+  </si>
+  <si>
+    <t>https://www.ocado.com/products/ocado-british-whole-milk-4-pints-78920011</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -255,7 +280,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -323,11 +348,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -340,6 +380,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1052,15 +1095,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="118" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="118" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1131,78 +1174,82 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="B2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+      <c r="B5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1228,53 +1275,39 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1303,53 +1336,39 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1378,53 +1397,39 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1453,53 +1458,39 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="A4" t="s">
         <v>56</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
+      <c r="A5" t="s">
         <v>58</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
+      <c r="A6" t="s">
         <v>50</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="A7" t="s">
         <v>52</v>
       </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="1" t="s">
+      <c r="A8" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
- Added Aldi - Updated README
</commit_message>
<xml_diff>
--- a/pricecomparison/pricewatch.xlsx
+++ b/pricecomparison/pricewatch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivek/Development/price-compare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96EC470F-E373-CB43-81FC-72A83A1E781C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{76DE53E2-F240-D741-8E2A-A523C2B3C9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sainsburys" sheetId="1" r:id="rId1"/>
@@ -18,10 +18,10 @@
     <sheet name="Asda" sheetId="3" r:id="rId3"/>
     <sheet name="Co-op" sheetId="4" r:id="rId4"/>
     <sheet name="Ocado" sheetId="5" r:id="rId5"/>
-    <sheet name="Morissons" sheetId="6" r:id="rId6"/>
-    <sheet name="Lidl" sheetId="7" r:id="rId7"/>
-    <sheet name="M&amp;S" sheetId="8" r:id="rId8"/>
-    <sheet name="Aldi" sheetId="9" r:id="rId9"/>
+    <sheet name="Aldi" sheetId="6" r:id="rId6"/>
+    <sheet name="Morissons" sheetId="7" r:id="rId7"/>
+    <sheet name="Lidl" sheetId="8" r:id="rId8"/>
+    <sheet name="M&amp;S" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="0"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="77">
   <si>
     <t>Product Name</t>
   </si>
@@ -227,19 +227,58 @@
   </si>
   <si>
     <t>https://www.ocado.com/products/ocado-british-whole-milk-4-pints-78920011</t>
+  </si>
+  <si>
+    <t>https://groceries.aldi.co.uk/en-GB/p-hovis-tasty-medium-sliced-wholemeal-bread-800g/5010003000339</t>
+  </si>
+  <si>
+    <t>Cowbelle Organic Semi Skimmed Milk 2.27 Litres / 4 Pints</t>
+  </si>
+  <si>
+    <t>https://groceries.aldi.co.uk/en-GB/p-cowbelle-organic-semi-skimmed-milk-227-litres-4-pints/4088600003719</t>
+  </si>
+  <si>
+    <t>1.55</t>
+  </si>
+  <si>
+    <t>Cowbelle Fresh British Whole Milk 2.27 Litres / 4 Pints</t>
+  </si>
+  <si>
+    <t>https://groceries.aldi.co.uk/en-GB/p-cowbelle-fresh-british-whole-milk-227-litres-4-pints/4088600003948</t>
+  </si>
+  <si>
+    <t>Cowbelle Fresh British Semi-skimmed Milk 3.41 Litres / 6 Pints</t>
+  </si>
+  <si>
+    <t>https://groceries.aldi.co.uk/en-GB/p-cowbelle-fresh-british-semi-skimmed-milk-341-litres-6-pints/4088600003887</t>
+  </si>
+  <si>
+    <t>Fairy Platinum Quickwash Original Washing Up Liquid 820.0</t>
+  </si>
+  <si>
+    <t>https://groceries.aldi.co.uk/en-GB/p-fairy-platinum-quickwash-original-washing-upliquid-8200/8001090430250</t>
+  </si>
+  <si>
+    <t>1.99</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -280,7 +319,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -363,12 +402,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -383,6 +436,10 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -707,18 +764,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="151.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="151.83203125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -885,18 +942,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.1640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -993,18 +1050,18 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="144.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="144.6640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1101,19 +1158,19 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="118" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="118" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1174,24 +1231,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="77.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.5" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1257,20 +1314,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="54" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1283,20 +1344,44 @@
       <c r="A3" t="s">
         <v>5</v>
       </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>67</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>70</v>
+      </c>
+      <c r="B5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1306,11 +1391,17 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>74</v>
+      </c>
+      <c r="B8" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1319,19 +1410,22 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47" style="6" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1380,19 +1474,22 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="47" style="6" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1447,13 +1544,13 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
- Added Morissons - Updated README
</commit_message>
<xml_diff>
--- a/pricecomparison/pricewatch.xlsx
+++ b/pricecomparison/pricewatch.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivek/Development/price-compare/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{76DE53E2-F240-D741-8E2A-A523C2B3C9C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{52F10445-3122-6349-BA56-AE61FBB883D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sainsburys" sheetId="1" r:id="rId1"/>
@@ -19,9 +19,10 @@
     <sheet name="Co-op" sheetId="4" r:id="rId4"/>
     <sheet name="Ocado" sheetId="5" r:id="rId5"/>
     <sheet name="Aldi" sheetId="6" r:id="rId6"/>
-    <sheet name="Morissons" sheetId="7" r:id="rId7"/>
+    <sheet name="Morrisons" sheetId="7" r:id="rId7"/>
     <sheet name="Lidl" sheetId="8" r:id="rId8"/>
     <sheet name="M&amp;S" sheetId="9" r:id="rId9"/>
+    <sheet name="B&amp;M" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="94">
   <si>
     <t>Product Name</t>
   </si>
@@ -260,19 +261,76 @@
   </si>
   <si>
     <t>1.99</t>
+  </si>
+  <si>
+    <t>Hovis Best of Both Medium Bread 750g</t>
+  </si>
+  <si>
+    <t>https://groceries.morrisons.com/products/hovis-best-of-both-medium-bread-121706011</t>
+  </si>
+  <si>
+    <t>Hovis Tasty Wholemeal Medium Bread 800g</t>
+  </si>
+  <si>
+    <t>https://groceries.morrisons.com/products/hovis-tasty-wholemeal-medium-bread-114318011</t>
+  </si>
+  <si>
+    <t>Morrisons British Semi Skimmed Milk 4 Pints</t>
+  </si>
+  <si>
+    <t>https://groceries.morrisons.com/products/morrisons-british-semi-skimmed-milk-4-pints-215937011</t>
+  </si>
+  <si>
+    <t>1.29</t>
+  </si>
+  <si>
+    <t>Morrisons British Whole Milk 4 Pints</t>
+  </si>
+  <si>
+    <t>https://groceries.morrisons.com/products/morrisons-british-whole-milk-4-pints-215811011</t>
+  </si>
+  <si>
+    <t>Morrisons British Semi Skimmed Milk 6 Pints</t>
+  </si>
+  <si>
+    <t>https://groceries.morrisons.com/products/morrisons-british-semi-skimmed-milk-6-pints-215941011</t>
+  </si>
+  <si>
+    <t>1.89</t>
+  </si>
+  <si>
+    <t>Morrisons British Whole Milk 6 Pints</t>
+  </si>
+  <si>
+    <t>https://groceries.morrisons.com/products/morrisons-british-whole-milk-6-pints-217959011</t>
+  </si>
+  <si>
+    <t>Fairy Washing Up Liquid Platinum Quickwash Original 820ml</t>
+  </si>
+  <si>
+    <t>https://groceries.morrisons.com/products/fairy-washing-up-liquid-platinum-quickwash-original-575130011</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -319,7 +377,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -417,11 +475,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -438,8 +511,11 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -764,8 +840,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="151.83203125" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="151.83203125" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -929,6 +1005,18 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -942,8 +1030,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.1640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1050,8 +1138,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="144.6640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="144.6640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1158,9 +1246,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="118" style="6" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="118" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.1640625" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1237,8 +1325,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" style="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="77.5" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.5" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1314,24 +1402,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="98" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="54" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1409,63 +1497,106 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>77</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>79</v>
+      </c>
+      <c r="B3" t="s">
+        <v>80</v>
+      </c>
+      <c r="C3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>81</v>
+      </c>
+      <c r="B4" t="s">
+        <v>82</v>
+      </c>
+      <c r="C4" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>84</v>
+      </c>
+      <c r="B5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C5" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>86</v>
+      </c>
+      <c r="B6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>89</v>
+      </c>
+      <c r="B7" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>91</v>
+      </c>
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" t="s">
+        <v>93</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -1479,7 +1610,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
- Excel Cleanup - Updated README
</commit_message>
<xml_diff>
--- a/pricecomparison/pricewatch.xlsx
+++ b/pricecomparison/pricewatch.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivek/Development/price-compare/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivek/Development/pricecomparison/pricecomparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{52F10445-3122-6349-BA56-AE61FBB883D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62585EFA-94BF-A043-8446-8D31931A57A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2800" yWindow="3700" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sainsburys" sheetId="1" r:id="rId1"/>
@@ -20,17 +20,13 @@
     <sheet name="Ocado" sheetId="5" r:id="rId5"/>
     <sheet name="Aldi" sheetId="6" r:id="rId6"/>
     <sheet name="Morrisons" sheetId="7" r:id="rId7"/>
-    <sheet name="Lidl" sheetId="8" r:id="rId8"/>
-    <sheet name="M&amp;S" sheetId="9" r:id="rId9"/>
-    <sheet name="B&amp;M" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="106">
   <si>
     <t>Product Name</t>
   </si>
@@ -212,22 +208,58 @@
     <t>https://api.shop.coop.co.uk/products/details/e3c61eda-a029-45ce-99f3-84ba9a8afa04?store_id=17eda196-0394-4cf5-9053-a7652fc76671</t>
   </si>
   <si>
+    <t>Fairy Original Washing Up Liquid Green with LiftAction 433 ML</t>
+  </si>
+  <si>
+    <t>https://api.shop.coop.co.uk/products/details/a9b87079-a5b1-4518-af6c-1786c484c19a?store_id=d8ad1898-e156-4c58-9386-f96d611d31eb</t>
+  </si>
+  <si>
+    <t>Hovis Tasty Wholemeal Medium Sliced Bread 800g</t>
+  </si>
+  <si>
     <t>https://www.ocado.com/products/hovis-tasty-wholemeal-medium-sliced-bread-15885011</t>
   </si>
   <si>
     <t>1.20</t>
   </si>
   <si>
-    <t>Hovis Tasty Wholemeal Medium Sliced Bread 800g</t>
-  </si>
-  <si>
     <t>Ocado British Semi Skimmed Milk 4 Pints</t>
   </si>
   <si>
     <t>https://www.ocado.com/products/ocado-british-semi-skimmed-milk-4-pints-78914011</t>
   </si>
   <si>
+    <t>Ocado British Whole Milk 4 Pints</t>
+  </si>
+  <si>
     <t>https://www.ocado.com/products/ocado-british-whole-milk-4-pints-78920011</t>
+  </si>
+  <si>
+    <t>M&amp;S Organic Semi-Skimmed Milk 4 Pints</t>
+  </si>
+  <si>
+    <t>https://www.ocado.com/products/m-s-organic-semi-skimmed-milk-4-pints-505327011</t>
+  </si>
+  <si>
+    <t>1.85</t>
+  </si>
+  <si>
+    <t>M&amp;S Select Farms British Whole Milk 4 Pints</t>
+  </si>
+  <si>
+    <t>https://www.ocado.com/products/m-s-select-farms-british-whole-milk-4-pints-505373011</t>
+  </si>
+  <si>
+    <t>1.30</t>
+  </si>
+  <si>
+    <t>Fairy Original Washing Up Liquid 780ml</t>
+  </si>
+  <si>
+    <t>https://www.ocado.com/products/fairy-original-washing-up-liquid-292135011</t>
+  </si>
+  <si>
+    <t>2.30</t>
   </si>
   <si>
     <t>https://groceries.aldi.co.uk/en-GB/p-hovis-tasty-medium-sliced-wholemeal-bread-800g/5010003000339</t>
@@ -1008,18 +1040,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C8"/>
@@ -1238,130 +1258,118 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="47" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="118" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="53.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="118.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2">
+        <v>1.5</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>58</v>
+      </c>
+      <c r="B3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C3">
+        <v>1.5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C4">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C5">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>54</v>
+        <v>1.35</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="77.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>62</v>
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -1369,28 +1377,35 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>58</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>72</v>
+      </c>
+      <c r="B6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C6" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>54</v>
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1400,10 +1415,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1413,79 +1428,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="B5" t="s">
-        <v>71</v>
+        <v>85</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>86</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>74</v>
-      </c>
-      <c r="B8" t="s">
-        <v>75</v>
-      </c>
-      <c r="C8" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -1497,230 +1502,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="91.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="51.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.5" style="7" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="5" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>92</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>98</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>89</v>
+        <v>101</v>
       </c>
       <c r="B7" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>91</v>
+        <v>103</v>
       </c>
       <c r="B8" t="s">
-        <v>92</v>
+        <v>104</v>
       </c>
       <c r="C8" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="47" style="7" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
-  <dimension ref="A1:C8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
- Refactored code - Introduced more tests - Introduced retries functionality, not across the stores - Fixed Adli & Morission's cookie related code - Fixed some of the Pylint identified issues
</commit_message>
<xml_diff>
--- a/pricecomparison/pricewatch.xlsx
+++ b/pricecomparison/pricewatch.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10608"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivek/Development/pricecomparison/pricecomparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62585EFA-94BF-A043-8446-8D31931A57A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:20001_{9385BEDF-9D1E-A843-BACC-EEA7777F1C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="3700" windowWidth="28040" windowHeight="17440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2800" yWindow="3700" windowWidth="28040" windowHeight="17440" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sainsburys" sheetId="1" r:id="rId1"/>
@@ -22,11 +22,12 @@
     <sheet name="Morrisons" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="107">
   <si>
     <t>Product Name</t>
   </si>
@@ -112,13 +113,13 @@
     <t>https://www.tesco.com/groceries/en-GB/products/261738730</t>
   </si>
   <si>
-    <t>1.00</t>
+    <t>1.10</t>
   </si>
   <si>
     <t>https://www.tesco.com/groceries/en-GB/products/255000362</t>
   </si>
   <si>
-    <t>1.10</t>
+    <t>1.20</t>
   </si>
   <si>
     <t>Tesco British Semi Skimmed Milk 2.272L 4 Pints</t>
@@ -127,7 +128,7 @@
     <t>https://www.tesco.com/groceries/en-GB/products/254656543</t>
   </si>
   <si>
-    <t>1.25</t>
+    <t>1.29</t>
   </si>
   <si>
     <t>Tesco Whole Milk 2.27L (4 pint)</t>
@@ -142,7 +143,7 @@
     <t>https://www.tesco.com/groceries/en-GB/products/255986260</t>
   </si>
   <si>
-    <t>1.70</t>
+    <t>1.89</t>
   </si>
   <si>
     <t>Tesco Whole Milk 3.4L (6 pint)</t>
@@ -172,6 +173,9 @@
     <t>https://groceries.asda.com/product/semi-skimmed-milk/asda-semi-skimmed-milk/20504</t>
   </si>
   <si>
+    <t>1.35</t>
+  </si>
+  <si>
     <t>Asda Whole Milk 2.27L (4 pint)</t>
   </si>
   <si>
@@ -184,6 +188,9 @@
     <t>https://groceries.asda.com/product/semi-skimmed-milk/asda-semi-skimmed-milk/20506</t>
   </si>
   <si>
+    <t>1.99</t>
+  </si>
+  <si>
     <t>Asda Whole Milk 3.4L (6 pint)</t>
   </si>
   <si>
@@ -196,6 +203,9 @@
     <t>https://groceries.asda.com/product/washing-up-liquid/fairy-platinum-quickwash-original-washing-up-liquid-with-up-to-3-x-faster-tough-grease-cleaning/1000360714103</t>
   </si>
   <si>
+    <t>Unnamed: 3</t>
+  </si>
+  <si>
     <t>Co Op British Fresh Semi-Skimmed Milk 4 Pints/2.272L</t>
   </si>
   <si>
@@ -220,15 +230,15 @@
     <t>https://www.ocado.com/products/hovis-tasty-wholemeal-medium-sliced-bread-15885011</t>
   </si>
   <si>
-    <t>1.20</t>
-  </si>
-  <si>
     <t>Ocado British Semi Skimmed Milk 4 Pints</t>
   </si>
   <si>
     <t>https://www.ocado.com/products/ocado-british-semi-skimmed-milk-4-pints-78914011</t>
   </si>
   <si>
+    <t>1.30</t>
+  </si>
+  <si>
     <t>Ocado British Whole Milk 4 Pints</t>
   </si>
   <si>
@@ -250,7 +260,7 @@
     <t>https://www.ocado.com/products/m-s-select-farms-british-whole-milk-4-pints-505373011</t>
   </si>
   <si>
-    <t>1.30</t>
+    <t>1.40</t>
   </si>
   <si>
     <t>Fairy Original Washing Up Liquid 780ml</t>
@@ -292,15 +302,15 @@
     <t>https://groceries.aldi.co.uk/en-GB/p-fairy-platinum-quickwash-original-washing-upliquid-8200/8001090430250</t>
   </si>
   <si>
-    <t>1.99</t>
-  </si>
-  <si>
     <t>Hovis Best of Both Medium Bread 750g</t>
   </si>
   <si>
     <t>https://groceries.morrisons.com/products/hovis-best-of-both-medium-bread-121706011</t>
   </si>
   <si>
+    <t>99p</t>
+  </si>
+  <si>
     <t>Hovis Tasty Wholemeal Medium Bread 800g</t>
   </si>
   <si>
@@ -313,9 +323,6 @@
     <t>https://groceries.morrisons.com/products/morrisons-british-semi-skimmed-milk-4-pints-215937011</t>
   </si>
   <si>
-    <t>1.29</t>
-  </si>
-  <si>
     <t>Morrisons British Whole Milk 4 Pints</t>
   </si>
   <si>
@@ -326,9 +333,6 @@
   </si>
   <si>
     <t>https://groceries.morrisons.com/products/morrisons-british-semi-skimmed-milk-6-pints-215941011</t>
-  </si>
-  <si>
-    <t>1.89</t>
   </si>
   <si>
     <t>Morrisons British Whole Milk 6 Pints</t>
@@ -350,25 +354,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -409,7 +401,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -492,41 +484,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -541,13 +503,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -867,23 +822,23 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="151.83203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="52.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="151.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -895,7 +850,7 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -906,7 +861,7 @@
         <v>6</v>
       </c>
       <c r="C3">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -917,7 +872,7 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -928,7 +883,7 @@
         <v>6</v>
       </c>
       <c r="C5">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -939,7 +894,7 @@
         <v>6</v>
       </c>
       <c r="C6">
-        <v>1.1000000000000001</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -950,7 +905,7 @@
         <v>4</v>
       </c>
       <c r="C7">
-        <v>1</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -961,7 +916,7 @@
         <v>12</v>
       </c>
       <c r="C8">
-        <v>2</v>
+        <v>1.75</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1036,7 +991,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1045,13 +999,13 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="54.1640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="54.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1144,7 +1098,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -1153,23 +1106,23 @@
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:C8"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="45.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="144.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="45.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="144.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1181,7 +1134,7 @@
         <v>44</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1203,48 +1156,48 @@
         <v>47</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" t="s">
         <v>48</v>
-      </c>
-      <c r="B5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C5" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B6" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" t="s">
         <v>53</v>
-      </c>
-      <c r="C7" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
         <v>43</v>
@@ -1252,63 +1205,75 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="53.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="118.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="C2">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1.55</v>
+      </c>
+      <c r="D2">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B3" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C3">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+        <v>1.55</v>
+      </c>
+      <c r="D3">
+        <v>1.55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="B4" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="C4">
+        <v>1.35</v>
+      </c>
+      <c r="D4">
         <v>1.35</v>
       </c>
     </row>
@@ -1321,91 +1286,90 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="43.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="77.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="B2" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C3" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="B7" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="C7" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -1417,14 +1381,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="54" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="98" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1443,7 +1404,7 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C2" t="s">
         <v>30</v>
@@ -1451,46 +1412,46 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B5" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>
@@ -1502,14 +1463,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="51.33203125" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="91.5" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -1525,79 +1485,79 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="C2" t="s">
-        <v>64</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C4" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B5" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C6" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B7" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C7" t="s">
-        <v>100</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B8" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C8" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Aldi's price retrieval code - Minor code fixes
</commit_message>
<xml_diff>
--- a/pricecomparison/pricewatch.xlsx
+++ b/pricecomparison/pricewatch.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6560" yWindow="4220" windowWidth="28040" windowHeight="17440" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6560" yWindow="4220" windowWidth="28040" windowHeight="17440" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sainsburys" sheetId="1" state="visible" r:id="rId1"/>
@@ -22,25 +22,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="6">
+  <fonts count="4">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="12"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <b val="1"/>
-      <sz val="12"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -66,42 +54,12 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -144,7 +102,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -153,12 +111,6 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -544,25 +496,25 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
@@ -820,25 +772,25 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
@@ -1004,22 +956,22 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
@@ -1185,22 +1137,22 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="4" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
@@ -1277,25 +1229,25 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
@@ -1441,22 +1393,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
@@ -1473,8 +1425,10 @@
           <t>https://groceries.aldi.co.uk/en-GB/p-hovis-tasty-medium-sliced-wholemeal-bread-800g/5010003000339</t>
         </is>
       </c>
-      <c r="C2" t="n">
-        <v>1.2</v>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>1.20</t>
+        </is>
       </c>
       <c r="D2" t="n">
         <v>1.2</v>
@@ -1491,6 +1445,11 @@
           <t>https://groceries.aldi.co.uk/en-GB/p-cowbelle-organic-semi-skimmed-milk-227-litres-4-pints/4088600003719</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>1.55</t>
+        </is>
+      </c>
       <c r="D3" t="n">
         <v>1.55</v>
       </c>
@@ -1506,6 +1465,11 @@
           <t>https://groceries.aldi.co.uk/en-GB/p-cowbelle-fresh-british-whole-milk-227-litres-4-pints/4088600003948</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>1.35</t>
+        </is>
+      </c>
       <c r="D4" t="n">
         <v>1.35</v>
       </c>
@@ -1521,6 +1485,11 @@
           <t>https://groceries.aldi.co.uk/en-GB/p-cowbelle-fresh-british-semi-skimmed-milk-341-litres-6-pints/4088600003887</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
+      </c>
       <c r="D5" t="n">
         <v>1.99</v>
       </c>
@@ -1536,8 +1505,10 @@
           <t>https://groceries.aldi.co.uk/en-GB/p-fairy-platinum-quickwash-original-washing-upliquid-8200/8001090430250</t>
         </is>
       </c>
-      <c r="C6" t="n">
-        <v>1.99</v>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>1.99</t>
+        </is>
       </c>
       <c r="D6" t="n">
         <v>1.99</v>
@@ -1560,25 +1531,25 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="5" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B1" s="5" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" s="5" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="5" t="inlineStr">
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>

</xml_diff>

<commit_message>
- Removed comments - Minor refactoring
</commit_message>
<xml_diff>
--- a/pricecomparison/pricewatch.xlsx
+++ b/pricecomparison/pricewatch.xlsx
@@ -496,25 +496,25 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
@@ -652,6 +652,9 @@
           <t>Sainsbury's Fairtrade Bananas x5</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr"/>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -659,6 +662,9 @@
           <t>Sainsbury's Whole Cucumber</t>
         </is>
       </c>
+      <c r="B10" t="inlineStr"/>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -666,6 +672,9 @@
           <t>Sainsbury's Mixed Peppers, SO Organic x3 (Colours may vary)</t>
         </is>
       </c>
+      <c r="B11" t="inlineStr"/>
+      <c r="C11" t="inlineStr"/>
+      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -673,6 +682,9 @@
           <t>Sainsbury's Strawberries 400g</t>
         </is>
       </c>
+      <c r="B12" t="inlineStr"/>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -680,6 +692,9 @@
           <t>Sainsbury's Easy Peelers, Taste the Difference 600g</t>
         </is>
       </c>
+      <c r="B13" t="inlineStr"/>
+      <c r="C13" t="inlineStr"/>
+      <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -687,6 +702,9 @@
           <t>Sainsbury's British Baby Potatoes 1kg</t>
         </is>
       </c>
+      <c r="B14" t="inlineStr"/>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -694,6 +712,9 @@
           <t>Sainsbury's Limes</t>
         </is>
       </c>
+      <c r="B15" t="inlineStr"/>
+      <c r="C15" t="inlineStr"/>
+      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -701,6 +722,9 @@
           <t>Sainsbury's Aubergine</t>
         </is>
       </c>
+      <c r="B16" t="inlineStr"/>
+      <c r="C16" t="inlineStr"/>
+      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -708,6 +732,9 @@
           <t>Sainsbury's Baby Button Mushrooms 200g</t>
         </is>
       </c>
+      <c r="B17" t="inlineStr"/>
+      <c r="C17" t="inlineStr"/>
+      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -715,6 +742,9 @@
           <t>Sainsbury's Young Spinach 260g</t>
         </is>
       </c>
+      <c r="B18" t="inlineStr"/>
+      <c r="C18" t="inlineStr"/>
+      <c r="D18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -722,6 +752,9 @@
           <t>Sainsbury's Root Ginger Loose</t>
         </is>
       </c>
+      <c r="B19" t="inlineStr"/>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -729,6 +762,9 @@
           <t>Sainsbury's Cherry Tomatoes 500g</t>
         </is>
       </c>
+      <c r="B20" t="inlineStr"/>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -736,6 +772,9 @@
           <t>Sainsbury's Fresh Packed Coriander 100g</t>
         </is>
       </c>
+      <c r="B21" t="inlineStr"/>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">

</xml_diff>

<commit_message>
-Enhanced logging - Moved hard-coded store names into an Enum
</commit_message>
<xml_diff>
--- a/pricecomparison/pricewatch.xlsx
+++ b/pricecomparison/pricewatch.xlsx
@@ -3,13 +3,13 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="6560" yWindow="4220" windowWidth="28040" windowHeight="17440" tabRatio="600" firstSheet="0" activeTab="5" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="7580" yWindow="5920" windowWidth="28040" windowHeight="17440" tabRatio="600" firstSheet="0" activeTab="3" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sainsburys" sheetId="1" state="visible" r:id="rId1"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tesco" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Asda" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Co-op" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Coop" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Ocado" sheetId="5" state="visible" r:id="rId5"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Aldi" sheetId="6" state="visible" r:id="rId6"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Morrisons" sheetId="7" state="visible" r:id="rId7"/>
@@ -22,13 +22,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="12"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -54,12 +60,27 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -102,7 +123,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -111,6 +132,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -499,22 +523,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
@@ -652,9 +676,6 @@
           <t>Sainsbury's Fairtrade Bananas x5</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr"/>
-      <c r="C9" t="inlineStr"/>
-      <c r="D9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -662,9 +683,6 @@
           <t>Sainsbury's Whole Cucumber</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr"/>
-      <c r="C10" t="inlineStr"/>
-      <c r="D10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -672,9 +690,6 @@
           <t>Sainsbury's Mixed Peppers, SO Organic x3 (Colours may vary)</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr"/>
-      <c r="C11" t="inlineStr"/>
-      <c r="D11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -682,9 +697,6 @@
           <t>Sainsbury's Strawberries 400g</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr"/>
-      <c r="C12" t="inlineStr"/>
-      <c r="D12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -692,9 +704,6 @@
           <t>Sainsbury's Easy Peelers, Taste the Difference 600g</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr"/>
-      <c r="C13" t="inlineStr"/>
-      <c r="D13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -702,9 +711,6 @@
           <t>Sainsbury's British Baby Potatoes 1kg</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr"/>
-      <c r="C14" t="inlineStr"/>
-      <c r="D14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -712,9 +718,6 @@
           <t>Sainsbury's Limes</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr"/>
-      <c r="C15" t="inlineStr"/>
-      <c r="D15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -722,9 +725,6 @@
           <t>Sainsbury's Aubergine</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
-      <c r="C16" t="inlineStr"/>
-      <c r="D16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -732,9 +732,6 @@
           <t>Sainsbury's Baby Button Mushrooms 200g</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
-      <c r="C17" t="inlineStr"/>
-      <c r="D17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -742,9 +739,6 @@
           <t>Sainsbury's Young Spinach 260g</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr"/>
-      <c r="C18" t="inlineStr"/>
-      <c r="D18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -752,9 +746,6 @@
           <t>Sainsbury's Root Ginger Loose</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr"/>
-      <c r="C19" t="inlineStr"/>
-      <c r="D19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -762,9 +753,6 @@
           <t>Sainsbury's Cherry Tomatoes 500g</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr"/>
-      <c r="C20" t="inlineStr"/>
-      <c r="D20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -772,9 +760,6 @@
           <t>Sainsbury's Fresh Packed Coriander 100g</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr"/>
-      <c r="C21" t="inlineStr"/>
-      <c r="D21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -811,25 +796,25 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
@@ -992,25 +977,25 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
@@ -1173,25 +1158,25 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
@@ -1268,25 +1253,25 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
@@ -1432,22 +1417,22 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="3" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>
@@ -1570,25 +1555,25 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>Product Name</t>
         </is>
       </c>
-      <c r="B1" s="2" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>URL</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>Price</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>Unnamed: 3</t>
         </is>

</xml_diff>

<commit_message>
- Added new store
</commit_message>
<xml_diff>
--- a/pricecomparison/pricewatch.xlsx
+++ b/pricecomparison/pricewatch.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vivek/Development/pricecomparison/pricecomparison/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A9171AD6-3CD6-DB4A-9EAB-DCED608293DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A2FCC522-14AA-3D4D-9812-CF0C7A4E8FD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7580" yWindow="5920" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,8 +18,9 @@
     <sheet name="Asda" sheetId="3" r:id="rId3"/>
     <sheet name="Coop" sheetId="4" r:id="rId4"/>
     <sheet name="Ocado" sheetId="5" r:id="rId5"/>
-    <sheet name="Aldi" sheetId="6" r:id="rId6"/>
-    <sheet name="Morrisons" sheetId="7" r:id="rId7"/>
+    <sheet name="WattsFarms" sheetId="6" r:id="rId6"/>
+    <sheet name="Aldi" sheetId="7" r:id="rId7"/>
+    <sheet name="Morrisons" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="0"/>
   <fileRecoveryPr repairLoad="1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="118">
   <si>
     <t>Product Name</t>
   </si>
@@ -276,6 +277,24 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>Kingsmill 50:50 Medium Bread</t>
+  </si>
+  <si>
+    <t>https://shop.wattsfarms.co.uk/products/hovis-best-of-both-loaf-800g</t>
+  </si>
+  <si>
+    <t>Milk Full Fat 2ltr</t>
+  </si>
+  <si>
+    <t>https://shop.wattsfarms.co.uk/collections/dairy-products-delivery/products/milk-full-fat-2ltr</t>
+  </si>
+  <si>
+    <t>Milk Semi-Skimmed 2ltr</t>
+  </si>
+  <si>
+    <t>https://shop.wattsfarms.co.uk/collections/dairy-products-delivery/products/milk-semi-skimmed-2ltr</t>
   </si>
   <si>
     <t>https://groceries.aldi.co.uk/en-GB/p-hovis-tasty-medium-sliced-wholemeal-bread-800g/5010003000339</t>
@@ -369,13 +388,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -398,7 +423,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -436,16 +461,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -764,7 +807,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -998,7 +1043,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5:C7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1519,14 +1566,79 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:E6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="54" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="98" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1552,7 +1664,7 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
@@ -1566,13 +1678,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>90</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
       <c r="D3">
         <v>1.2</v>
@@ -1583,10 +1695,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>87</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>88</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -1600,10 +1712,10 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>89</v>
+        <v>95</v>
       </c>
       <c r="B5" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="C5" t="s">
         <v>41</v>
@@ -1617,13 +1729,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>91</v>
+        <v>97</v>
       </c>
       <c r="B6" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="D6">
         <v>1.2</v>
@@ -1634,11 +1746,12 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1668,27 +1781,27 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
+        <v>101</v>
       </c>
       <c r="C2" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="D2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
       <c r="E2" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>98</v>
+        <v>104</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>105</v>
       </c>
       <c r="C3" t="s">
         <v>36</v>
@@ -1702,10 +1815,10 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B4" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -1714,15 +1827,15 @@
         <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="B5" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
@@ -1731,15 +1844,15 @@
         <v>35</v>
       </c>
       <c r="E5" t="s">
-        <v>102</v>
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>111</v>
       </c>
       <c r="B6" t="s">
-        <v>106</v>
+        <v>112</v>
       </c>
       <c r="C6" t="s">
         <v>41</v>
@@ -1748,15 +1861,15 @@
         <v>41</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>107</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
-        <v>108</v>
+        <v>114</v>
       </c>
       <c r="C7" t="s">
         <v>41</v>
@@ -1765,21 +1878,21 @@
         <v>41</v>
       </c>
       <c r="E7" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="B8" t="s">
-        <v>110</v>
+        <v>116</v>
       </c>
       <c r="D8" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="E8" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>